<commit_message>
Debug: Test des secrets dans le workflow
</commit_message>
<xml_diff>
--- a/liste.xlsx
+++ b/liste.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PYTHON\envoi_email_sans_piece_jointe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\envoimails\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2BFCFC-A802-4CFB-95ED-24B1ED79DFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEE35EA-A63A-446C-B8E7-F63975E4F868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27165" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{2FCAF40A-FD52-43CB-BAF8-6650B29623A3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2FCAF40A-FD52-43CB-BAF8-6650B29623A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Reçus Fiscaux 2023" sheetId="1" r:id="rId1"/>
@@ -126,16 +126,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;\ _€_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="00"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="167" formatCode="[$-40C]d\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="168" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="0000000000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -176,12 +175,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -264,9 +257,9 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -330,11 +323,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Euro" xfId="3" xr:uid="{437BBEC9-DDC9-41E3-A381-5A07D09411CC}"/>
@@ -659,10 +647,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB213"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A274" sqref="A5:XFD274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -887,633 +875,6 @@
       <c r="AA4" s="17"/>
       <c r="AB4" s="17"/>
     </row>
-    <row r="5" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L5" s="24"/>
-    </row>
-    <row r="6" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L6" s="24"/>
-    </row>
-    <row r="7" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L7" s="24"/>
-    </row>
-    <row r="8" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L8" s="24"/>
-    </row>
-    <row r="9" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L9" s="24"/>
-    </row>
-    <row r="10" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L10" s="24"/>
-    </row>
-    <row r="11" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L11" s="24"/>
-    </row>
-    <row r="12" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L12" s="24"/>
-    </row>
-    <row r="13" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L13" s="24"/>
-    </row>
-    <row r="14" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L14" s="24"/>
-    </row>
-    <row r="15" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L15" s="24"/>
-    </row>
-    <row r="16" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L16" s="24"/>
-    </row>
-    <row r="17" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L17" s="24"/>
-    </row>
-    <row r="18" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L18" s="24"/>
-    </row>
-    <row r="19" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L19" s="24"/>
-    </row>
-    <row r="20" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L20" s="24"/>
-    </row>
-    <row r="21" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L21" s="24"/>
-    </row>
-    <row r="22" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L22" s="24"/>
-    </row>
-    <row r="23" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L23" s="24"/>
-    </row>
-    <row r="24" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L24" s="24"/>
-    </row>
-    <row r="25" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L25" s="24"/>
-    </row>
-    <row r="26" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L26" s="24"/>
-    </row>
-    <row r="27" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L27" s="24"/>
-    </row>
-    <row r="28" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L28" s="26"/>
-    </row>
-    <row r="29" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L29" s="24"/>
-    </row>
-    <row r="30" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L30" s="24"/>
-    </row>
-    <row r="31" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L31" s="24"/>
-    </row>
-    <row r="32" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L32" s="24"/>
-    </row>
-    <row r="33" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L33" s="24"/>
-    </row>
-    <row r="34" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L34" s="24"/>
-    </row>
-    <row r="35" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L35" s="24"/>
-    </row>
-    <row r="36" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L36" s="24"/>
-    </row>
-    <row r="37" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L37" s="24"/>
-    </row>
-    <row r="38" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L38" s="24"/>
-    </row>
-    <row r="39" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L39" s="27"/>
-    </row>
-    <row r="40" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L40" s="24"/>
-    </row>
-    <row r="41" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L41" s="24"/>
-    </row>
-    <row r="42" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L42" s="24"/>
-    </row>
-    <row r="43" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L43" s="24"/>
-    </row>
-    <row r="44" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L44" s="24"/>
-    </row>
-    <row r="45" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L45" s="24"/>
-    </row>
-    <row r="46" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L46" s="24"/>
-    </row>
-    <row r="47" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L47" s="24"/>
-    </row>
-    <row r="48" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L48" s="24"/>
-    </row>
-    <row r="49" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L49" s="24"/>
-    </row>
-    <row r="50" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L50" s="24"/>
-    </row>
-    <row r="51" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L51" s="24"/>
-    </row>
-    <row r="52" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L52" s="24"/>
-    </row>
-    <row r="53" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L53" s="24"/>
-    </row>
-    <row r="54" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L54" s="24"/>
-    </row>
-    <row r="55" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L55" s="24"/>
-    </row>
-    <row r="56" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L56" s="24"/>
-    </row>
-    <row r="57" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L57" s="24"/>
-    </row>
-    <row r="58" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L58" s="24"/>
-    </row>
-    <row r="59" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L59" s="24"/>
-    </row>
-    <row r="60" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L60" s="24"/>
-    </row>
-    <row r="61" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L61" s="24"/>
-    </row>
-    <row r="62" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L62" s="24"/>
-    </row>
-    <row r="63" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L63" s="24"/>
-    </row>
-    <row r="64" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L64" s="24"/>
-    </row>
-    <row r="65" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L65" s="24"/>
-    </row>
-    <row r="66" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L66" s="24"/>
-    </row>
-    <row r="67" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L67" s="24"/>
-    </row>
-    <row r="68" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L68" s="24"/>
-    </row>
-    <row r="69" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L69" s="24"/>
-    </row>
-    <row r="70" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L70" s="24"/>
-    </row>
-    <row r="71" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L71" s="24"/>
-    </row>
-    <row r="72" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L72" s="24"/>
-    </row>
-    <row r="73" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L73" s="24"/>
-    </row>
-    <row r="74" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L74" s="24"/>
-    </row>
-    <row r="75" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L75" s="24"/>
-    </row>
-    <row r="76" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L76" s="24"/>
-    </row>
-    <row r="77" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L77" s="24"/>
-    </row>
-    <row r="78" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L78" s="24"/>
-    </row>
-    <row r="79" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L79" s="24"/>
-    </row>
-    <row r="80" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L80" s="24"/>
-    </row>
-    <row r="81" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L81" s="24"/>
-    </row>
-    <row r="82" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L82" s="24"/>
-    </row>
-    <row r="83" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L83" s="24"/>
-    </row>
-    <row r="84" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L84" s="24"/>
-    </row>
-    <row r="85" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L85" s="24"/>
-    </row>
-    <row r="86" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L86" s="26"/>
-    </row>
-    <row r="87" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L87" s="24"/>
-    </row>
-    <row r="88" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L88" s="24"/>
-    </row>
-    <row r="89" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L89" s="24"/>
-    </row>
-    <row r="90" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L90" s="24"/>
-    </row>
-    <row r="91" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L91" s="24"/>
-    </row>
-    <row r="92" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L92" s="24"/>
-    </row>
-    <row r="93" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L93" s="24"/>
-    </row>
-    <row r="94" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L94" s="24"/>
-    </row>
-    <row r="95" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L95" s="24"/>
-    </row>
-    <row r="96" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L96" s="24"/>
-    </row>
-    <row r="97" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L97" s="24"/>
-    </row>
-    <row r="98" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L98" s="24"/>
-    </row>
-    <row r="99" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L99" s="24"/>
-    </row>
-    <row r="100" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L100" s="24"/>
-    </row>
-    <row r="101" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L101" s="24"/>
-    </row>
-    <row r="102" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L102" s="24"/>
-    </row>
-    <row r="103" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L103" s="24"/>
-    </row>
-    <row r="104" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L104" s="24"/>
-    </row>
-    <row r="105" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L105" s="24"/>
-    </row>
-    <row r="106" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L106" s="24"/>
-    </row>
-    <row r="107" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L107" s="24"/>
-    </row>
-    <row r="108" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L108" s="24"/>
-    </row>
-    <row r="109" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L109" s="24"/>
-    </row>
-    <row r="110" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L110" s="24"/>
-    </row>
-    <row r="111" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L111" s="24"/>
-    </row>
-    <row r="112" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L112" s="24"/>
-    </row>
-    <row r="113" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L113" s="24"/>
-    </row>
-    <row r="114" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L114" s="24"/>
-    </row>
-    <row r="115" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L115" s="24"/>
-    </row>
-    <row r="116" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L116" s="24"/>
-    </row>
-    <row r="117" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L117" s="24"/>
-    </row>
-    <row r="118" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L118" s="24"/>
-    </row>
-    <row r="119" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L119" s="24"/>
-    </row>
-    <row r="120" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L120" s="24"/>
-    </row>
-    <row r="121" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L121" s="24"/>
-    </row>
-    <row r="122" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L122" s="24"/>
-    </row>
-    <row r="123" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L123" s="24"/>
-    </row>
-    <row r="124" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L124" s="24"/>
-    </row>
-    <row r="125" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L125" s="24"/>
-    </row>
-    <row r="126" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L126" s="24"/>
-    </row>
-    <row r="127" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L127" s="24"/>
-    </row>
-    <row r="128" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L128" s="24"/>
-    </row>
-    <row r="129" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L129" s="24"/>
-    </row>
-    <row r="130" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L130" s="24"/>
-    </row>
-    <row r="131" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L131" s="24"/>
-    </row>
-    <row r="132" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L132" s="24"/>
-    </row>
-    <row r="133" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L133" s="24"/>
-    </row>
-    <row r="134" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L134" s="24"/>
-    </row>
-    <row r="135" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L135" s="24"/>
-    </row>
-    <row r="136" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L136" s="24"/>
-    </row>
-    <row r="137" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L137" s="24"/>
-    </row>
-    <row r="138" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L138" s="24"/>
-    </row>
-    <row r="139" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L139" s="24"/>
-    </row>
-    <row r="140" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L140" s="24"/>
-    </row>
-    <row r="141" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L141" s="24"/>
-    </row>
-    <row r="142" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L142" s="24"/>
-    </row>
-    <row r="143" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L143" s="24"/>
-    </row>
-    <row r="144" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L144" s="24"/>
-    </row>
-    <row r="145" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L145" s="24"/>
-    </row>
-    <row r="146" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L146" s="24"/>
-    </row>
-    <row r="147" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L147" s="24"/>
-    </row>
-    <row r="148" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L148" s="24"/>
-    </row>
-    <row r="149" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L149" s="24"/>
-    </row>
-    <row r="150" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L150" s="24"/>
-    </row>
-    <row r="151" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L151" s="24"/>
-    </row>
-    <row r="152" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L152" s="24"/>
-    </row>
-    <row r="153" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L153" s="24"/>
-    </row>
-    <row r="154" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L154" s="24"/>
-    </row>
-    <row r="155" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L155" s="24"/>
-    </row>
-    <row r="156" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L156" s="24"/>
-    </row>
-    <row r="157" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L157" s="24"/>
-    </row>
-    <row r="158" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L158" s="24"/>
-    </row>
-    <row r="159" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L159" s="24"/>
-    </row>
-    <row r="160" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L160" s="24"/>
-    </row>
-    <row r="161" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L161" s="24"/>
-    </row>
-    <row r="162" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L162" s="24"/>
-    </row>
-    <row r="163" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L163" s="24"/>
-    </row>
-    <row r="164" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L164" s="24"/>
-    </row>
-    <row r="165" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L165" s="24"/>
-    </row>
-    <row r="166" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L166" s="24"/>
-    </row>
-    <row r="167" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L167" s="24"/>
-    </row>
-    <row r="168" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L168" s="24"/>
-    </row>
-    <row r="169" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L169" s="24"/>
-    </row>
-    <row r="170" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L170" s="24"/>
-    </row>
-    <row r="171" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L171" s="24"/>
-    </row>
-    <row r="172" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L172" s="26"/>
-    </row>
-    <row r="173" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L173" s="24"/>
-    </row>
-    <row r="174" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L174" s="24"/>
-    </row>
-    <row r="175" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L175" s="24"/>
-    </row>
-    <row r="176" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L176" s="26"/>
-    </row>
-    <row r="177" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L177" s="24"/>
-    </row>
-    <row r="178" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L178" s="24"/>
-    </row>
-    <row r="179" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L179" s="24"/>
-    </row>
-    <row r="180" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L180" s="24"/>
-    </row>
-    <row r="181" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L181" s="24"/>
-    </row>
-    <row r="182" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L182" s="24"/>
-    </row>
-    <row r="183" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L183" s="24"/>
-    </row>
-    <row r="184" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L184" s="24"/>
-    </row>
-    <row r="185" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L185" s="24"/>
-    </row>
-    <row r="186" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L186" s="24"/>
-    </row>
-    <row r="187" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L187" s="24"/>
-    </row>
-    <row r="188" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L188" s="24"/>
-    </row>
-    <row r="189" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L189" s="24"/>
-    </row>
-    <row r="190" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L190" s="24"/>
-    </row>
-    <row r="191" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L191" s="24"/>
-    </row>
-    <row r="192" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L192" s="24"/>
-    </row>
-    <row r="193" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L193" s="25"/>
-    </row>
-    <row r="194" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L194" s="24"/>
-    </row>
-    <row r="195" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L195" s="24"/>
-    </row>
-    <row r="196" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L196" s="24"/>
-    </row>
-    <row r="197" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L197" s="24"/>
-    </row>
-    <row r="198" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L198" s="24"/>
-    </row>
-    <row r="199" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L199" s="24"/>
-    </row>
-    <row r="200" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L200" s="24"/>
-    </row>
-    <row r="201" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L201" s="24"/>
-    </row>
-    <row r="202" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L202" s="24"/>
-    </row>
-    <row r="203" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L203" s="24"/>
-    </row>
-    <row r="204" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L204" s="24"/>
-    </row>
-    <row r="205" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L205" s="24"/>
-    </row>
-    <row r="206" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L206" s="24"/>
-    </row>
-    <row r="207" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L207" s="24"/>
-    </row>
-    <row r="208" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L208" s="24"/>
-    </row>
-    <row r="209" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L209" s="24"/>
-    </row>
-    <row r="210" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L210" s="24"/>
-    </row>
-    <row r="211" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L211" s="24"/>
-    </row>
-    <row r="212" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L212" s="24"/>
-    </row>
-    <row r="213" spans="12:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L213" s="24"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" xr:uid="{4789A97C-A179-4E97-B22C-3453C2C118DE}"/>

</xml_diff>